<commit_message>
Exercicio modulo 04 corrigido
</commit_message>
<xml_diff>
--- a/Exercicios/Modulo 04 - Técnicas de testes/Planilhas do exercicio - modulo 04.xlsx
+++ b/Exercicios/Modulo 04 - Técnicas de testes/Planilhas do exercicio - modulo 04.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="495" windowWidth="20775" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="495" windowWidth="20730" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Exercicio 01" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,7 @@
     <sheet name="Exercicio 03" sheetId="3" r:id="rId3"/>
     <sheet name="RN04" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataSignature="AMtx7mgdh7l7PLCyc/y+B8+0PgttyccUgg=="/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>RN01 - Os valores dos produtos devem estar entre R$ 19,00 e R$ 99,00</t>
   </si>
@@ -35,9 +34,6 @@
   </si>
   <si>
     <t>Cadastrar valor R$ 40,00---&gt; válido</t>
-  </si>
-  <si>
-    <t>Cadastrar valor R$99,00 ---&gt; válido</t>
   </si>
   <si>
     <t>Cadastrar valor R$ 120,00 ---&gt; inválido</t>
@@ -53,9 +49,6 @@
   </si>
   <si>
     <t>22 dias ---&gt; não renovar</t>
-  </si>
-  <si>
-    <t>30 dias ---&gt; não renovar</t>
   </si>
   <si>
     <t>40 dias ---&gt; renovar</t>
@@ -425,23 +418,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -464,7 +445,6 @@
     <xf numFmtId="8" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -481,15 +461,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +616,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>278686</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>199670</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="695325" cy="266700"/>
@@ -682,7 +675,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>392986</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>180620</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="397589" cy="266700"/>
@@ -1153,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:N997"/>
+  <dimension ref="D2:N993"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1168,89 +1161,89 @@
   <sheetData>
     <row r="2" spans="4:14" ht="15" customHeight="1" thickBot="1"/>
     <row r="3" spans="4:14">
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="4:14" ht="15.75" thickBot="1">
-      <c r="D4" s="21"/>
-      <c r="E4" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="22"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="4:14" ht="15.75" thickTop="1">
-      <c r="D5" s="21"/>
-      <c r="E5" s="23" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="22"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="21"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="22"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="21"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="4:14">
-      <c r="D8" s="21"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="22"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="18"/>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="21"/>
-      <c r="E9" s="25"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="22"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="21"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="2"/>
@@ -1258,436 +1251,389 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="22"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="21"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="38">
+      <c r="D11" s="17"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="32">
         <v>10</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="36">
+      <c r="G11" s="20"/>
+      <c r="H11" s="30">
         <v>40</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="36">
+      <c r="J11" s="30">
         <v>120</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="22"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="4:14">
-      <c r="D12" s="21"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="21"/>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="21"/>
-      <c r="E14" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="22"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="21"/>
-      <c r="E15" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="22"/>
-    </row>
-    <row r="16" spans="4:14">
-      <c r="D16" s="30"/>
-      <c r="E16" s="28" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="31"/>
-    </row>
-    <row r="17" spans="4:12">
-      <c r="D17" s="30"/>
-      <c r="E17" s="28" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="4:14" ht="15.75" thickBot="1">
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+    </row>
+    <row r="17" spans="4:12" ht="15" customHeight="1" thickBot="1"/>
+    <row r="18" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D19" s="17"/>
+      <c r="E19" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="4:12" ht="15.75" customHeight="1" thickTop="1">
+      <c r="D20" s="17"/>
+      <c r="E20" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="31"/>
-    </row>
-    <row r="18" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="34"/>
-    </row>
-    <row r="19" spans="4:12" ht="15" customHeight="1" thickBot="1"/>
-    <row r="20" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D21" s="21"/>
-      <c r="E21" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="22"/>
-    </row>
-    <row r="22" spans="4:12" ht="15.75" customHeight="1" thickTop="1">
-      <c r="D22" s="21"/>
-      <c r="E22" s="16" t="s">
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D21" s="17"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D24" s="17"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D25" s="17"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="18"/>
+    </row>
+    <row r="26" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="22"/>
-    </row>
-    <row r="23" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D23" s="21"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="22"/>
-    </row>
-    <row r="24" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D24" s="21"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="22"/>
-    </row>
-    <row r="25" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D25" s="21"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="22"/>
-    </row>
-    <row r="26" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D26" s="21"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="22"/>
+      <c r="H26" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="33"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D27" s="21"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="22"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="18"/>
     </row>
     <row r="28" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D28" s="21"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="37" t="s">
+      <c r="D28" s="17"/>
+      <c r="E28" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="40"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="18"/>
     </row>
     <row r="29" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D29" s="21"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="22"/>
-    </row>
-    <row r="30" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D30" s="21"/>
-      <c r="E30" s="28" t="s">
+      <c r="D29" s="17"/>
+      <c r="E29" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="22"/>
-    </row>
-    <row r="31" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D31" s="21"/>
-      <c r="E31" s="28" t="s">
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="28"/>
+    </row>
+    <row r="31" spans="4:12" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="32" spans="4:12" ht="15.75" customHeight="1">
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="4:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D33" s="17"/>
+      <c r="E33" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="4:11" ht="15.75" customHeight="1" thickTop="1">
+      <c r="D34" s="17"/>
+      <c r="E34" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="22"/>
-    </row>
-    <row r="32" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D32" s="21"/>
-      <c r="E32" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="22"/>
-    </row>
-    <row r="33" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D33" s="32"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="34"/>
-    </row>
-    <row r="34" spans="4:12" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="35" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D35" s="18"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D35" s="17"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D36" s="21"/>
-      <c r="E36" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="22"/>
-    </row>
-    <row r="37" spans="4:12" ht="15.75" customHeight="1" thickTop="1">
-      <c r="D37" s="21"/>
-      <c r="E37" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="22"/>
-    </row>
-    <row r="38" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D38" s="21"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="22"/>
-    </row>
-    <row r="39" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D39" s="21"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="22"/>
-    </row>
-    <row r="40" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D40" s="21"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="22"/>
-    </row>
-    <row r="41" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D41" s="21"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="22"/>
-    </row>
-    <row r="42" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D42" s="21"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="22"/>
-    </row>
-    <row r="43" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D43" s="21"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="44">
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D36" s="17"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D37" s="17"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D38" s="17"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D39" s="17"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D40" s="17"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="37">
         <v>80</v>
       </c>
-      <c r="H43" s="37">
+      <c r="H40" s="31">
         <v>115</v>
       </c>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="22"/>
-    </row>
-    <row r="44" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D44" s="21"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="22"/>
-    </row>
-    <row r="45" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D45" s="21"/>
-      <c r="E45" s="28" t="s">
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D41" s="17"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D42" s="17"/>
+      <c r="E42" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="4:11" ht="15.75" customHeight="1">
+      <c r="D43" s="17"/>
+      <c r="E43" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="22"/>
-    </row>
-    <row r="46" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D46" s="21"/>
-      <c r="E46" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="22"/>
-    </row>
-    <row r="47" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D47" s="21"/>
-      <c r="E47" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="22"/>
-    </row>
-    <row r="48" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="34"/>
-    </row>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="18"/>
+    </row>
+    <row r="44" spans="4:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="28"/>
+    </row>
+    <row r="45" spans="4:11" ht="15.75" customHeight="1"/>
+    <row r="46" spans="4:11" ht="15.75" customHeight="1"/>
+    <row r="47" spans="4:11" ht="15.75" customHeight="1"/>
+    <row r="48" spans="4:11" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2633,18 +2579,14 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E34:J34"/>
     <mergeCell ref="E4:K4"/>
     <mergeCell ref="E5:K5"/>
-    <mergeCell ref="E21:K21"/>
-    <mergeCell ref="E22:K22"/>
-    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E19:K19"/>
+    <mergeCell ref="E20:K20"/>
+    <mergeCell ref="E33:J33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2672,89 +2614,89 @@
   <sheetData>
     <row r="2" spans="4:14" ht="15" customHeight="1" thickBot="1"/>
     <row r="3" spans="4:14">
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="4:14" ht="15.75" thickBot="1">
-      <c r="D4" s="21"/>
-      <c r="E4" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="22"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="4:14" ht="15.75" thickTop="1">
-      <c r="D5" s="21"/>
-      <c r="E5" s="23" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="22"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="21"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="22"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="21"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="4:14">
-      <c r="D8" s="21"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="22"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="18"/>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="21"/>
-      <c r="E9" s="25"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="22"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="21"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="2"/>
@@ -2762,281 +2704,281 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="22"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="21"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="38">
+      <c r="D11" s="17"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="32">
         <v>18.989999999999998</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="30">
         <v>19.010000000000002</v>
       </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="38">
+      <c r="H11" s="37"/>
+      <c r="I11" s="32">
         <v>98.99</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J11" s="30">
         <v>99.01</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="22"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="4:14">
-      <c r="D12" s="21"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="21"/>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="4:14">
+      <c r="D14" s="17"/>
+      <c r="E14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="4:14">
+      <c r="D15" s="17"/>
+      <c r="E15" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="4:14">
+      <c r="D16" s="24"/>
+      <c r="E16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="22"/>
-    </row>
-    <row r="14" spans="4:14">
-      <c r="D14" s="21"/>
-      <c r="E14" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="22"/>
-    </row>
-    <row r="15" spans="4:14">
-      <c r="D15" s="21"/>
-      <c r="E15" s="28" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="4:12">
+      <c r="D17" s="24"/>
+      <c r="E17" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="22"/>
-    </row>
-    <row r="16" spans="4:14">
-      <c r="D16" s="30"/>
-      <c r="E16" s="28" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="4:12">
+      <c r="D18" s="24"/>
+      <c r="E18" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="31"/>
-    </row>
-    <row r="17" spans="4:12">
-      <c r="D17" s="30"/>
-      <c r="E17" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="31"/>
-    </row>
-    <row r="18" spans="4:12">
-      <c r="D18" s="30"/>
-      <c r="E18" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="31"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D19" s="32"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="34"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="28"/>
     </row>
     <row r="21" spans="4:12" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="22" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="20"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D23" s="21"/>
-      <c r="E23" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="22"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="4:12" ht="15.75" customHeight="1" thickTop="1">
-      <c r="D24" s="21"/>
-      <c r="E24" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="22"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D25" s="21"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="22"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="18"/>
     </row>
     <row r="26" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D26" s="21"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="22"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="18"/>
     </row>
     <row r="27" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D27" s="21"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="22"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D28" s="21"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="22"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D29" s="21"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="1"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="22"/>
+      <c r="K29" s="18"/>
     </row>
     <row r="30" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D30" s="21"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="44">
+      <c r="D30" s="17"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="37">
         <v>99</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="31">
         <v>101</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="22"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D31" s="21"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="22"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="18"/>
     </row>
     <row r="32" spans="4:12" ht="15.75" customHeight="1">
-      <c r="D32" s="21"/>
-      <c r="E32" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="22"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="18"/>
     </row>
     <row r="33" spans="4:11" ht="15.75" customHeight="1">
-      <c r="D33" s="21"/>
-      <c r="E33" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="22"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="18"/>
     </row>
     <row r="34" spans="4:11" ht="15.75" customHeight="1">
-      <c r="D34" s="21"/>
-      <c r="E34" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="22"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="18"/>
     </row>
     <row r="35" spans="4:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="34"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
     </row>
     <row r="36" spans="4:11" ht="15.75" customHeight="1"/>
     <row r="37" spans="4:11" ht="15.75" customHeight="1"/>
@@ -4017,184 +3959,184 @@
   <sheetData>
     <row r="2" spans="4:12" ht="15" customHeight="1" thickBot="1"/>
     <row r="3" spans="4:12">
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D4" s="21"/>
-      <c r="E4" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="45"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="4:12" ht="15.75" thickTop="1">
-      <c r="D5" s="21"/>
-      <c r="E5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="22"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="4:12">
-      <c r="D6" s="21"/>
-      <c r="E6" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="22"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="4:12">
-      <c r="D7" s="21"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="4:12">
-      <c r="D8" s="21"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="46"/>
+      <c r="J8" s="39"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="4:12">
-      <c r="D9" s="21"/>
-      <c r="E9" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="44">
+      <c r="D9" s="17"/>
+      <c r="E9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="37">
         <v>1</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="37">
         <v>1</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="37">
         <v>0</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="37">
         <v>0</v>
       </c>
-      <c r="J9" s="45"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="4:12">
-      <c r="D10" s="21"/>
-      <c r="E10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="44">
+      <c r="D10" s="17"/>
+      <c r="E10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="37">
         <v>1</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="37">
         <v>0</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="37">
         <v>1</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="37">
         <v>0</v>
       </c>
-      <c r="J10" s="45"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="4:12">
-      <c r="D11" s="21"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="45"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="4:12">
-      <c r="D12" s="21"/>
-      <c r="E12" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="44">
+      <c r="D12" s="17"/>
+      <c r="E12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="37">
         <v>1</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="37">
         <v>1</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="37">
         <v>0</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="37">
         <v>0</v>
       </c>
-      <c r="J12" s="45"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="4:12">
-      <c r="D13" s="21"/>
-      <c r="E13" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="44">
+      <c r="D13" s="17"/>
+      <c r="E13" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="37">
         <v>1</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="37">
         <v>0</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="37">
         <v>1</v>
       </c>
-      <c r="I13" s="44">
+      <c r="I13" s="37">
         <v>0</v>
       </c>
-      <c r="J13" s="45"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="4:12" ht="15" customHeight="1" thickBot="1">
-      <c r="D14" s="42"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="43"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="17" spans="13:13">
       <c r="M17" s="10"/>
@@ -5207,7 +5149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -5218,234 +5160,234 @@
   <sheetData>
     <row r="2" spans="4:21" ht="15" customHeight="1" thickBot="1"/>
     <row r="3" spans="4:21">
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D4" s="21"/>
-      <c r="E4" s="50" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="4:21" ht="15.75" thickTop="1">
+      <c r="D5" s="17"/>
+      <c r="E5" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="4:21">
+      <c r="D6" s="17"/>
+      <c r="E6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="22"/>
-    </row>
-    <row r="5" spans="4:21" ht="15.75" thickTop="1">
-      <c r="D5" s="21"/>
-      <c r="E5" s="23" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="4:21">
+      <c r="D7" s="17"/>
+      <c r="E7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="22"/>
-    </row>
-    <row r="6" spans="4:21">
-      <c r="D6" s="21"/>
-      <c r="E6" s="25" t="s">
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="18"/>
+    </row>
+    <row r="8" spans="4:21">
+      <c r="D8" s="17"/>
+      <c r="E8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="4:21">
-      <c r="D7" s="21"/>
-      <c r="E7" s="25" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="18"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+    </row>
+    <row r="9" spans="4:21">
+      <c r="D9" s="17"/>
+      <c r="E9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="4:21">
-      <c r="D8" s="21"/>
-      <c r="E8" s="25" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="4:21">
+      <c r="D10" s="17"/>
+      <c r="E10" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="22"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-    </row>
-    <row r="9" spans="4:21">
-      <c r="D9" s="21"/>
-      <c r="E9" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="4:21">
-      <c r="D10" s="21"/>
-      <c r="E10" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="22"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="4:21">
-      <c r="D11" s="21"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="22"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="4:21">
-      <c r="D12" s="21"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="4:21">
-      <c r="D13" s="21"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="4:21">
-      <c r="D14" s="21"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="22"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="4:21">
-      <c r="D15" s="21"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="22"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="4:21">
-      <c r="D16" s="21"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="22"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="4:12">
-      <c r="D17" s="21"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="22"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="4:12">
-      <c r="D18" s="21"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="22"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="4:12">
-      <c r="D19" s="21"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="22"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="4:12">
-      <c r="D20" s="21"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="22"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="4:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D21" s="42"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="43"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="36"/>
     </row>
     <row r="22" spans="4:12" ht="15.75" customHeight="1"/>
     <row r="23" spans="4:12" ht="15.75" customHeight="1"/>

</xml_diff>